<commit_message>
Combined Dalton and Terry's designs
</commit_message>
<xml_diff>
--- a/Party pig calendar.xlsx
+++ b/Party pig calendar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dvoth/Documents/Github/party-pig-html/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FB61846-8F62-9C47-8752-3E923D0D9FCE}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54BE3E9B-9BFB-534A-A675-04F1B9B4CC53}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8280" yWindow="460" windowWidth="25300" windowHeight="18080" tabRatio="788" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -214,7 +214,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -257,7 +257,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -345,7 +351,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyFill="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyFill="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="top"/>
     </xf>
@@ -398,13 +404,19 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="13" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
+    <xf numFmtId="164" fontId="14" fillId="7" borderId="0" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="7" borderId="0" xfId="12" applyFont="1" applyFill="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="15" applyFill="1"/>
-    <xf numFmtId="0" fontId="13" fillId="2" borderId="0" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="0" xfId="11">
       <alignment horizontal="left" vertical="top" wrapText="1" indent="1"/>
     </xf>
@@ -414,10 +426,16 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="5" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="7" borderId="0" xfId="12" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="left" indent="1"/>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="0" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="14" fillId="8" borderId="0" xfId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -426,14 +444,11 @@
     <xf numFmtId="0" fontId="15" fillId="8" borderId="0" xfId="13" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="7" borderId="0" xfId="12" applyFont="1" applyFill="1">
-      <alignment horizontal="left" indent="1"/>
+    <xf numFmtId="164" fontId="14" fillId="9" borderId="0" xfId="13" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1">
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" xfId="13" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="17">
@@ -895,7 +910,7 @@
   <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15"/>
@@ -910,49 +925,49 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="1" customFormat="1" ht="60" customHeight="1">
-      <c r="A1" s="20" t="str">
+      <c r="A1" s="26" t="str">
         <f ca="1">"January "&amp;CalendarYear</f>
         <v>January 2018</v>
       </c>
-      <c r="B1" s="20"/>
-      <c r="C1" s="20"/>
-      <c r="D1" s="20"/>
-      <c r="E1" s="20"/>
-      <c r="F1" s="20"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="J1" s="19" t="s">
+      <c r="B1" s="26"/>
+      <c r="C1" s="26"/>
+      <c r="D1" s="26"/>
+      <c r="E1" s="26"/>
+      <c r="F1" s="26"/>
+      <c r="G1" s="26"/>
+      <c r="H1" s="26"/>
+      <c r="J1" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="K1" s="19"/>
+      <c r="K1" s="22"/>
     </row>
     <row r="2" spans="1:11" s="2" customFormat="1" ht="21.75" customHeight="1">
-      <c r="A2" s="18"/>
-      <c r="B2" s="30" t="str">
+      <c r="A2" s="27"/>
+      <c r="B2" s="28" t="str">
         <f>WeekStart</f>
         <v>SUNDAY</v>
       </c>
-      <c r="C2" s="30" t="str">
+      <c r="C2" s="28" t="str">
         <f t="shared" ref="C2:H2" ca="1" si="0">UPPER(TEXT(C3,"dddd"))</f>
         <v>MONDAY</v>
       </c>
-      <c r="D2" s="30" t="str">
+      <c r="D2" s="28" t="str">
         <f ca="1">UPPER(TEXT(D3,"dddd"))</f>
         <v>TUESDAY</v>
       </c>
-      <c r="E2" s="30" t="str">
+      <c r="E2" s="28" t="str">
         <f t="shared" ca="1" si="0"/>
         <v>WEDNESDAY</v>
       </c>
-      <c r="F2" s="30" t="str">
+      <c r="F2" s="28" t="str">
         <f t="shared" ca="1" si="0"/>
         <v>THURSDAY</v>
       </c>
-      <c r="G2" s="30" t="str">
+      <c r="G2" s="28" t="str">
         <f t="shared" ca="1" si="0"/>
         <v>FRIDAY</v>
       </c>
-      <c r="H2" s="30" t="str">
+      <c r="H2" s="28" t="str">
         <f t="shared" ca="1" si="0"/>
         <v>SATURDAY</v>
       </c>
@@ -965,32 +980,32 @@
       </c>
     </row>
     <row r="3" spans="1:11" s="5" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A3" s="18"/>
-      <c r="B3" s="24">
+      <c r="A3" s="27"/>
+      <c r="B3" s="18">
         <f t="array" aca="1" ref="B3:H3" ca="1">DaysAndWeeks+DATE(CalendarYear,1,1)-WEEKDAY(DATE(CalendarYear,1,1),(WeekStart="Monday")+1)+1</f>
         <v>43100</v>
       </c>
-      <c r="C3" s="24">
+      <c r="C3" s="18">
         <f ca="1"/>
         <v>43101</v>
       </c>
-      <c r="D3" s="24">
+      <c r="D3" s="18">
         <f ca="1"/>
         <v>43102</v>
       </c>
-      <c r="E3" s="24">
+      <c r="E3" s="18">
         <f ca="1"/>
         <v>43103</v>
       </c>
-      <c r="F3" s="24">
+      <c r="F3" s="18">
         <f ca="1"/>
         <v>43104</v>
       </c>
-      <c r="G3" s="24">
+      <c r="G3" s="18">
         <f ca="1"/>
         <v>43105</v>
       </c>
-      <c r="H3" s="24">
+      <c r="H3" s="18">
         <f ca="1"/>
         <v>43106</v>
       </c>
@@ -1002,183 +1017,183 @@
       </c>
     </row>
     <row r="4" spans="1:11" ht="40" customHeight="1">
-      <c r="A4" s="18"/>
-      <c r="B4" s="25"/>
-      <c r="C4" s="25"/>
-      <c r="D4" s="25"/>
-      <c r="E4" s="25"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="25"/>
-      <c r="H4" s="25"/>
+      <c r="A4" s="27"/>
+      <c r="B4" s="19"/>
+      <c r="C4" s="19"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19"/>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
       <c r="I4" s="14"/>
       <c r="J4" s="15"/>
       <c r="K4" s="14"/>
     </row>
     <row r="5" spans="1:11" s="5" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A5" s="12"/>
-      <c r="B5" s="26">
+      <c r="A5" s="29"/>
+      <c r="B5" s="30">
         <f t="array" aca="1" ref="B5:H5" ca="1">DaysAndWeeks+DATE(CalendarYear,1,1)-WEEKDAY(DATE(CalendarYear,1,1),(WeekStart="Monday")+1)+8</f>
         <v>43107</v>
       </c>
-      <c r="C5" s="26">
+      <c r="C5" s="30">
         <f ca="1"/>
         <v>43108</v>
       </c>
-      <c r="D5" s="26">
+      <c r="D5" s="30">
         <f ca="1"/>
         <v>43109</v>
       </c>
-      <c r="E5" s="26">
+      <c r="E5" s="30">
         <f ca="1"/>
         <v>43110</v>
       </c>
-      <c r="F5" s="26">
+      <c r="F5" s="30">
         <f ca="1"/>
         <v>43111</v>
       </c>
-      <c r="G5" s="26">
+      <c r="G5" s="30">
         <f ca="1"/>
         <v>43112</v>
       </c>
-      <c r="H5" s="26">
+      <c r="H5" s="32">
         <f ca="1"/>
         <v>43113</v>
       </c>
     </row>
     <row r="6" spans="1:11" s="8" customFormat="1" ht="40" customHeight="1">
-      <c r="A6" s="12"/>
-      <c r="B6" s="27"/>
-      <c r="C6" s="27"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="27"/>
-      <c r="G6" s="27"/>
-      <c r="H6" s="27"/>
+      <c r="A6" s="29"/>
+      <c r="B6" s="31"/>
+      <c r="C6" s="31"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="31"/>
+      <c r="G6" s="31"/>
+      <c r="H6" s="33"/>
       <c r="J6" s="9"/>
     </row>
     <row r="7" spans="1:11" s="5" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A7" s="12"/>
-      <c r="B7" s="28">
+      <c r="A7" s="29"/>
+      <c r="B7" s="20">
         <f t="array" aca="1" ref="B7:H7" ca="1">DaysAndWeeks+DATE(CalendarYear,1,1)-WEEKDAY(DATE(CalendarYear,1,1),(WeekStart="Monday")+1)+15</f>
         <v>43114</v>
       </c>
-      <c r="C7" s="28">
+      <c r="C7" s="20">
         <f ca="1"/>
         <v>43115</v>
       </c>
-      <c r="D7" s="28">
+      <c r="D7" s="20">
         <f ca="1"/>
         <v>43116</v>
       </c>
-      <c r="E7" s="28">
+      <c r="E7" s="20">
         <f ca="1"/>
         <v>43117</v>
       </c>
-      <c r="F7" s="28">
+      <c r="F7" s="20">
         <f ca="1"/>
         <v>43118</v>
       </c>
-      <c r="G7" s="28">
+      <c r="G7" s="20">
         <f ca="1"/>
         <v>43119</v>
       </c>
-      <c r="H7" s="28">
+      <c r="H7" s="20">
         <f ca="1"/>
         <v>43120</v>
       </c>
       <c r="J7" s="6"/>
     </row>
     <row r="8" spans="1:11" s="8" customFormat="1" ht="40" customHeight="1">
-      <c r="A8" s="12"/>
-      <c r="B8" s="29"/>
-      <c r="C8" s="29"/>
-      <c r="D8" s="29"/>
-      <c r="E8" s="29"/>
-      <c r="F8" s="29"/>
-      <c r="G8" s="29"/>
-      <c r="H8" s="29"/>
+      <c r="A8" s="29"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="21"/>
     </row>
     <row r="9" spans="1:11" s="5" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A9" s="12"/>
-      <c r="B9" s="26">
+      <c r="A9" s="29"/>
+      <c r="B9" s="30">
         <f t="array" aca="1" ref="B9:H9" ca="1">DaysAndWeeks+DATE(CalendarYear,1,1)-WEEKDAY(DATE(CalendarYear,1,1),(WeekStart="Monday")+1)+22</f>
         <v>43121</v>
       </c>
-      <c r="C9" s="26">
+      <c r="C9" s="30">
         <f ca="1"/>
         <v>43122</v>
       </c>
-      <c r="D9" s="26">
+      <c r="D9" s="30">
         <f ca="1"/>
         <v>43123</v>
       </c>
-      <c r="E9" s="26">
+      <c r="E9" s="30">
         <f ca="1"/>
         <v>43124</v>
       </c>
-      <c r="F9" s="26">
+      <c r="F9" s="30">
         <f ca="1"/>
         <v>43125</v>
       </c>
-      <c r="G9" s="26">
+      <c r="G9" s="30">
         <f ca="1"/>
         <v>43126</v>
       </c>
-      <c r="H9" s="26">
+      <c r="H9" s="30">
         <f ca="1"/>
         <v>43127</v>
       </c>
     </row>
     <row r="10" spans="1:11" s="8" customFormat="1" ht="40" customHeight="1">
-      <c r="A10" s="12"/>
-      <c r="B10" s="27"/>
-      <c r="C10" s="27"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="27"/>
-      <c r="F10" s="27"/>
-      <c r="G10" s="27"/>
-      <c r="H10" s="27"/>
+      <c r="A10" s="29"/>
+      <c r="B10" s="31"/>
+      <c r="C10" s="31"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="31"/>
+      <c r="H10" s="31"/>
     </row>
     <row r="11" spans="1:11" s="5" customFormat="1" ht="19.5" customHeight="1">
-      <c r="A11" s="12"/>
-      <c r="B11" s="28">
+      <c r="A11" s="29"/>
+      <c r="B11" s="20">
         <f t="array" aca="1" ref="B11:H11" ca="1">DaysAndWeeks+DATE(CalendarYear,1,1)-WEEKDAY(DATE(CalendarYear,1,1),(WeekStart="Monday")+1)+29</f>
         <v>43128</v>
       </c>
-      <c r="C11" s="28">
+      <c r="C11" s="20">
         <f ca="1"/>
         <v>43129</v>
       </c>
-      <c r="D11" s="28">
+      <c r="D11" s="20">
         <f ca="1"/>
         <v>43130</v>
       </c>
-      <c r="E11" s="28">
+      <c r="E11" s="20">
         <f ca="1"/>
         <v>43131</v>
       </c>
-      <c r="F11" s="28">
+      <c r="F11" s="20">
         <f ca="1"/>
         <v>43132</v>
       </c>
-      <c r="G11" s="28">
+      <c r="G11" s="20">
         <f ca="1"/>
         <v>43133</v>
       </c>
-      <c r="H11" s="28">
+      <c r="H11" s="20">
         <f ca="1"/>
         <v>43134</v>
       </c>
     </row>
     <row r="12" spans="1:11" s="8" customFormat="1" ht="40" customHeight="1">
-      <c r="A12" s="12"/>
-      <c r="B12" s="29"/>
-      <c r="C12" s="29"/>
-      <c r="D12" s="29"/>
-      <c r="E12" s="29"/>
-      <c r="F12" s="29"/>
-      <c r="G12" s="29"/>
-      <c r="H12" s="29"/>
+      <c r="A12" s="29"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="21"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="21"/>
+      <c r="G12" s="21"/>
+      <c r="H12" s="21"/>
     </row>
     <row r="13" spans="1:11" s="5" customFormat="1" ht="19.5" customHeight="1">
       <c r="A13" s="12"/>
@@ -1253,12 +1268,12 @@
   <sheetData>
     <row r="1" spans="1:8" ht="60" customHeight="1">
       <c r="A1" s="14"/>
-      <c r="B1" s="23" t="str">
+      <c r="B1" s="25" t="str">
         <f ca="1">"October "&amp;CalendarYear</f>
         <v>October 2018</v>
       </c>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
@@ -1510,23 +1525,23 @@
         <f ca="1"/>
         <v>43409</v>
       </c>
-      <c r="D13" s="21" t="s">
+      <c r="D13" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="E13" s="22"/>
-      <c r="F13" s="22"/>
-      <c r="G13" s="22"/>
-      <c r="H13" s="22"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="24"/>
     </row>
     <row r="14" spans="1:8" ht="58" customHeight="1">
       <c r="A14" s="14"/>
       <c r="B14" s="17"/>
       <c r="C14" s="17"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="22"/>
-      <c r="G14" s="22"/>
-      <c r="H14" s="22"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1583,12 +1598,12 @@
   <sheetData>
     <row r="1" spans="1:8" ht="60" customHeight="1">
       <c r="A1" s="14"/>
-      <c r="B1" s="23" t="str">
+      <c r="B1" s="25" t="str">
         <f ca="1">"November "&amp;CalendarYear</f>
         <v>November 2018</v>
       </c>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
@@ -1840,23 +1855,23 @@
         <f ca="1"/>
         <v>43437</v>
       </c>
-      <c r="D13" s="21" t="s">
+      <c r="D13" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="E13" s="22"/>
-      <c r="F13" s="22"/>
-      <c r="G13" s="22"/>
-      <c r="H13" s="22"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="24"/>
     </row>
     <row r="14" spans="1:8" ht="58" customHeight="1">
       <c r="A14" s="14"/>
       <c r="B14" s="17"/>
       <c r="C14" s="17"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="22"/>
-      <c r="G14" s="22"/>
-      <c r="H14" s="22"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -1913,12 +1928,12 @@
   <sheetData>
     <row r="1" spans="1:8" ht="60" customHeight="1">
       <c r="A1" s="14"/>
-      <c r="B1" s="23" t="str">
+      <c r="B1" s="25" t="str">
         <f ca="1">"December "&amp;CalendarYear</f>
         <v>December 2018</v>
       </c>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
@@ -2170,23 +2185,23 @@
         <f ca="1"/>
         <v>43465</v>
       </c>
-      <c r="D13" s="21" t="s">
+      <c r="D13" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="E13" s="22"/>
-      <c r="F13" s="22"/>
-      <c r="G13" s="22"/>
-      <c r="H13" s="22"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="24"/>
     </row>
     <row r="14" spans="1:8" ht="58" customHeight="1">
       <c r="A14" s="14"/>
       <c r="B14" s="17"/>
       <c r="C14" s="17"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="22"/>
-      <c r="G14" s="22"/>
-      <c r="H14" s="22"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2244,12 +2259,12 @@
   <sheetData>
     <row r="1" spans="1:8" s="1" customFormat="1" ht="60" customHeight="1">
       <c r="A1" s="12"/>
-      <c r="B1" s="23" t="str">
+      <c r="B1" s="25" t="str">
         <f ca="1">"February "&amp;CalendarYear</f>
         <v>February 2018</v>
       </c>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
@@ -2496,22 +2511,22 @@
         <f ca="1"/>
         <v>43164</v>
       </c>
-      <c r="D13" s="21" t="s">
+      <c r="D13" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="E13" s="22"/>
-      <c r="F13" s="22"/>
-      <c r="G13" s="22"/>
-      <c r="H13" s="22"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="24"/>
     </row>
     <row r="14" spans="1:8" ht="58" customHeight="1">
       <c r="B14" s="17"/>
       <c r="C14" s="17"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="22"/>
-      <c r="G14" s="22"/>
-      <c r="H14" s="22"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2569,12 +2584,12 @@
   <sheetData>
     <row r="1" spans="1:8" ht="60" customHeight="1">
       <c r="A1" s="14"/>
-      <c r="B1" s="23" t="str">
+      <c r="B1" s="25" t="str">
         <f ca="1">"March "&amp;CalendarYear</f>
         <v>March 2018</v>
       </c>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
@@ -2826,23 +2841,23 @@
         <f ca="1"/>
         <v>43192</v>
       </c>
-      <c r="D13" s="21" t="s">
+      <c r="D13" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="E13" s="22"/>
-      <c r="F13" s="22"/>
-      <c r="G13" s="22"/>
-      <c r="H13" s="22"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="24"/>
     </row>
     <row r="14" spans="1:8" ht="58" customHeight="1">
       <c r="A14" s="14"/>
       <c r="B14" s="17"/>
       <c r="C14" s="17"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="22"/>
-      <c r="G14" s="22"/>
-      <c r="H14" s="22"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2900,12 +2915,12 @@
   <sheetData>
     <row r="1" spans="1:8" ht="60" customHeight="1">
       <c r="A1" s="14"/>
-      <c r="B1" s="23" t="str">
+      <c r="B1" s="25" t="str">
         <f ca="1">"April "&amp;CalendarYear</f>
         <v>April 2018</v>
       </c>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
@@ -3157,23 +3172,23 @@
         <f ca="1"/>
         <v>43227</v>
       </c>
-      <c r="D13" s="21" t="s">
+      <c r="D13" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="E13" s="22"/>
-      <c r="F13" s="22"/>
-      <c r="G13" s="22"/>
-      <c r="H13" s="22"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="24"/>
     </row>
     <row r="14" spans="1:8" ht="58" customHeight="1">
       <c r="A14" s="14"/>
       <c r="B14" s="17"/>
       <c r="C14" s="17"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="22"/>
-      <c r="G14" s="22"/>
-      <c r="H14" s="22"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -3231,12 +3246,12 @@
   <sheetData>
     <row r="1" spans="1:8" ht="60" customHeight="1">
       <c r="A1" s="14"/>
-      <c r="B1" s="23" t="str">
+      <c r="B1" s="25" t="str">
         <f ca="1">"May "&amp;CalendarYear</f>
         <v>May 2018</v>
       </c>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
@@ -3488,23 +3503,23 @@
         <f ca="1"/>
         <v>43255</v>
       </c>
-      <c r="D13" s="21" t="s">
+      <c r="D13" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="E13" s="22"/>
-      <c r="F13" s="22"/>
-      <c r="G13" s="22"/>
-      <c r="H13" s="22"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="24"/>
     </row>
     <row r="14" spans="1:8" ht="58" customHeight="1">
       <c r="A14" s="14"/>
       <c r="B14" s="17"/>
       <c r="C14" s="17"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="22"/>
-      <c r="G14" s="22"/>
-      <c r="H14" s="22"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -3562,12 +3577,12 @@
   <sheetData>
     <row r="1" spans="1:8" ht="60" customHeight="1">
       <c r="A1" s="14"/>
-      <c r="B1" s="23" t="str">
+      <c r="B1" s="25" t="str">
         <f ca="1">"June "&amp;CalendarYear</f>
         <v>June 2018</v>
       </c>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
@@ -3819,23 +3834,23 @@
         <f ca="1"/>
         <v>43283</v>
       </c>
-      <c r="D13" s="21" t="s">
+      <c r="D13" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="E13" s="22"/>
-      <c r="F13" s="22"/>
-      <c r="G13" s="22"/>
-      <c r="H13" s="22"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="24"/>
     </row>
     <row r="14" spans="1:8" ht="58" customHeight="1">
       <c r="A14" s="14"/>
       <c r="B14" s="17"/>
       <c r="C14" s="17"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="22"/>
-      <c r="G14" s="22"/>
-      <c r="H14" s="22"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -3893,12 +3908,12 @@
   <sheetData>
     <row r="1" spans="1:8" ht="60" customHeight="1">
       <c r="A1" s="14"/>
-      <c r="B1" s="23" t="str">
+      <c r="B1" s="25" t="str">
         <f ca="1">"July "&amp;CalendarYear</f>
         <v>July 2018</v>
       </c>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
@@ -4150,23 +4165,23 @@
         <f ca="1"/>
         <v>43318</v>
       </c>
-      <c r="D13" s="21" t="s">
+      <c r="D13" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="E13" s="22"/>
-      <c r="F13" s="22"/>
-      <c r="G13" s="22"/>
-      <c r="H13" s="22"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="24"/>
     </row>
     <row r="14" spans="1:8" ht="58" customHeight="1">
       <c r="A14" s="14"/>
       <c r="B14" s="17"/>
       <c r="C14" s="17"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="22"/>
-      <c r="G14" s="22"/>
-      <c r="H14" s="22"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -4224,12 +4239,12 @@
   <sheetData>
     <row r="1" spans="1:8" ht="60" customHeight="1">
       <c r="A1" s="14"/>
-      <c r="B1" s="23" t="str">
+      <c r="B1" s="25" t="str">
         <f ca="1">"August "&amp;CalendarYear</f>
         <v>August 2018</v>
       </c>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
@@ -4481,23 +4496,23 @@
         <f ca="1"/>
         <v>43346</v>
       </c>
-      <c r="D13" s="21" t="s">
+      <c r="D13" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="E13" s="22"/>
-      <c r="F13" s="22"/>
-      <c r="G13" s="22"/>
-      <c r="H13" s="22"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="24"/>
     </row>
     <row r="14" spans="1:8" ht="58" customHeight="1">
       <c r="A14" s="14"/>
       <c r="B14" s="17"/>
       <c r="C14" s="17"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="22"/>
-      <c r="G14" s="22"/>
-      <c r="H14" s="22"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -4555,12 +4570,12 @@
   <sheetData>
     <row r="1" spans="1:8" ht="60" customHeight="1">
       <c r="A1" s="14"/>
-      <c r="B1" s="23" t="str">
+      <c r="B1" s="25" t="str">
         <f ca="1">"September "&amp;CalendarYear</f>
         <v>September 2018</v>
       </c>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
@@ -4812,23 +4827,23 @@
         <f ca="1"/>
         <v>43374</v>
       </c>
-      <c r="D13" s="21" t="s">
+      <c r="D13" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="E13" s="22"/>
-      <c r="F13" s="22"/>
-      <c r="G13" s="22"/>
-      <c r="H13" s="22"/>
+      <c r="E13" s="24"/>
+      <c r="F13" s="24"/>
+      <c r="G13" s="24"/>
+      <c r="H13" s="24"/>
     </row>
     <row r="14" spans="1:8" ht="58" customHeight="1">
       <c r="A14" s="14"/>
       <c r="B14" s="17"/>
       <c r="C14" s="17"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="22"/>
-      <c r="G14" s="22"/>
-      <c r="H14" s="22"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="24"/>
+      <c r="F14" s="24"/>
+      <c r="G14" s="24"/>
+      <c r="H14" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>